<commit_message>
edit index and login htmls
</commit_message>
<xml_diff>
--- a/lineup_app/static/xlgap.xlsx
+++ b/lineup_app/static/xlgap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="516" windowWidth="16188" windowHeight="5376" activeTab="2"/>
+    <workbookView xWindow="132" yWindow="516" windowWidth="16188" windowHeight="5376" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="connections2" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">connections2!$A$2:$H$303</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1800,11 +1799,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="217904640"/>
-        <c:axId val="217906176"/>
+        <c:axId val="219289472"/>
+        <c:axId val="219291008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="217904640"/>
+        <c:axId val="219289472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,12 +1813,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217906176"/>
+        <c:crossAx val="219291008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="217906176"/>
+        <c:axId val="219291008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,7 +1829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217904640"/>
+        <c:crossAx val="219289472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10365,8 +10364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10449,7 +10448,7 @@
         <v>KPC</v>
       </c>
       <c r="D2">
-        <f>E2+F2</f>
+        <f t="shared" ref="D2:D66" si="0">E2+F2</f>
         <v>150</v>
       </c>
       <c r="E2">
@@ -10517,7 +10516,7 @@
         <v>U2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D66" si="0">E3+F3</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E3">
@@ -18703,7 +18702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
started looking at show ref case on results page
</commit_message>
<xml_diff>
--- a/lineup_app/static/xlgap.xlsx
+++ b/lineup_app/static/xlgap.xlsx
@@ -10365,7 +10365,7 @@
   <dimension ref="A1:T124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10517,35 +10517,35 @@
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>230</v>
       </c>
       <c r="E3">
         <v>80</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="G3">
         <v>501</v>
       </c>
       <c r="H3">
         <f>IF(M3*D3^3+N3*D3^2+O3*D3+P3&lt;0,0,M3*D3^3+N3*D3^2+O3*D3+P3)</f>
-        <v>734.39999999999964</v>
+        <v>190.39999999999964</v>
       </c>
       <c r="I3">
         <f>H3*G3/1000</f>
-        <v>367.93439999999981</v>
+        <v>95.390399999999815</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J66" si="1">IF(Q3*D3^3+R3*D3^2+S3*D3+T3&lt;0,0,Q3*D3^3+R3*D3^2+S3*D3+T3)</f>
-        <v>322.08</v>
+        <v>360.03</v>
       </c>
       <c r="K3">
         <v>500</v>
       </c>
       <c r="L3">
         <f>K3-J3</f>
-        <v>177.92000000000002</v>
+        <v>139.97000000000003</v>
       </c>
       <c r="M3">
         <v>-1.3333333333333263E-4</v>
@@ -18756,11 +18756,11 @@
       </c>
       <c r="B3" s="35">
         <f>SUMIF(Wells!$C$2:$C$200,A3,Wells!$H$2:$H$200)</f>
-        <v>21297.599999999999</v>
+        <v>20753.599999999999</v>
       </c>
       <c r="C3" s="35">
         <f>SUMIF(Wells!$C$2:$C$200,A3,Wells!$I$2:$I$200)</f>
-        <v>11579.284799999996</v>
+        <v>11306.740799999996</v>
       </c>
       <c r="D3" s="35">
         <v>79</v>
@@ -18796,11 +18796,11 @@
       </c>
       <c r="B5" s="36">
         <f>SUM(B2:B4)</f>
-        <v>88172.800000000047</v>
+        <v>87628.800000000047</v>
       </c>
       <c r="C5" s="36">
         <f>SUM(C2:C4)</f>
-        <v>49534.563199999975</v>
+        <v>49262.019199999966</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5">

</xml_diff>

<commit_message>
finished ref case saving logic
</commit_message>
<xml_diff>
--- a/lineup_app/static/xlgap.xlsx
+++ b/lineup_app/static/xlgap.xlsx
@@ -1799,11 +1799,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="205723520"/>
-        <c:axId val="205725056"/>
+        <c:axId val="220993408"/>
+        <c:axId val="220994944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="205723520"/>
+        <c:axId val="220993408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1813,12 +1813,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205725056"/>
+        <c:crossAx val="220994944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205725056"/>
+        <c:axId val="220994944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1829,7 +1829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205723520"/>
+        <c:crossAx val="220993408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2177,7 +2177,7 @@
   <dimension ref="A1:I303"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10366,7 +10366,7 @@
   <dimension ref="A1:T124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10442,43 +10442,43 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" t="str">
         <f>IF(B2="",VLOOKUP(A2,connections2!$A$3:$I$378,3,FALSE),VLOOKUP(B2,connections2!$G$3:$I$378,3,FALSE))</f>
-        <v>U2</v>
+        <v>KPC</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D66" si="0">E2+F2</f>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>500</v>
       </c>
       <c r="H2">
         <f>IF(M2*D2^3+N2*D2^2+O2*D2+P2&lt;0,0,M2*D2^3+N2*D2^2+O2*D2+P2)</f>
-        <v>599.99999999999932</v>
+        <v>699.99999999999966</v>
       </c>
       <c r="I2">
         <f>H2*G2/1000</f>
-        <v>299.99999999999966</v>
+        <v>349.99999999999983</v>
       </c>
       <c r="J2">
         <f>IF(Q2*D2^3+R2*D2^2+S2*D2+T2&lt;0,0,Q2*D2^3+R2*D2^2+S2*D2+T2)</f>
-        <v>348.75</v>
+        <v>330</v>
       </c>
       <c r="K2">
         <v>500</v>
       </c>
       <c r="L2">
         <f>K2-J2</f>
-        <v>151.25</v>
+        <v>170</v>
       </c>
       <c r="M2">
         <v>-1.3333333333333263E-4</v>
@@ -10518,35 +10518,35 @@
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E3">
         <v>80</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>501</v>
       </c>
       <c r="H3">
         <f>IF(M3*D3^3+N3*D3^2+O3*D3+P3&lt;0,0,M3*D3^3+N3*D3^2+O3*D3+P3)</f>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I3">
         <f>H3*G3/1000</f>
-        <v>323.84639999999973</v>
+        <v>367.93439999999981</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J66" si="1">IF(Q3*D3^3+R3*D3^2+S3*D3+T3&lt;0,0,Q3*D3^3+R3*D3^2+S3*D3+T3)</f>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K3">
         <v>500</v>
       </c>
       <c r="L3">
         <f>K3-J3</f>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M3">
         <v>-1.3333333333333263E-4</v>
@@ -10578,43 +10578,43 @@
         <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C4" t="str">
         <f>IF(B4="",VLOOKUP(A4,connections2!$A$3:$I$378,3,FALSE),VLOOKUP(B4,connections2!$G$3:$I$378,3,FALSE))</f>
-        <v>U2</v>
+        <v>U3</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E4">
         <v>80</v>
       </c>
       <c r="F4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>502</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H66" si="2">IF(M4*D4^3+N4*D4^2+O4*D4+P4&lt;0,0,M4*D4^3+N4*D4^2+O4*D4+P4)</f>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I66" si="3">H4*G4/1000</f>
-        <v>324.49279999999976</v>
+        <v>368.66879999999981</v>
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K4">
         <v>500</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L66" si="4">K4-J4</f>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M4">
         <v>-1.3333333333333263E-4</v>
@@ -10654,35 +10654,35 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E5">
         <v>80</v>
       </c>
       <c r="F5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>503</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>325.13919999999979</v>
+        <v>369.40319999999986</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K5">
         <v>500</v>
       </c>
       <c r="L5">
         <f t="shared" si="4"/>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M5">
         <v>-1.3333333333333263E-4</v>
@@ -10719,35 +10719,35 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="E6">
         <v>130</v>
       </c>
       <c r="F6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>504</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>498.39999999999952</v>
+        <v>646.39999999999952</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>251.19359999999978</v>
+        <v>325.78559999999976</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>356.88</v>
+        <v>341.73</v>
       </c>
       <c r="K6">
         <v>500</v>
       </c>
       <c r="L6">
         <f t="shared" si="4"/>
-        <v>143.12</v>
+        <v>158.26999999999998</v>
       </c>
       <c r="M6">
         <v>-1.3333333333333263E-4</v>
@@ -10787,35 +10787,35 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E7">
         <v>80</v>
       </c>
       <c r="F7">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>505</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>326.43199999999979</v>
+        <v>370.87199999999984</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K7">
         <v>500</v>
       </c>
       <c r="L7">
         <f t="shared" si="4"/>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M7">
         <v>-1.3333333333333263E-4</v>
@@ -10852,35 +10852,35 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="E8">
         <v>130</v>
       </c>
       <c r="F8">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>506</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>498.39999999999952</v>
+        <v>646.39999999999952</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>252.19039999999976</v>
+        <v>327.07839999999976</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>356.88</v>
+        <v>341.73</v>
       </c>
       <c r="K8">
         <v>500</v>
       </c>
       <c r="L8">
         <f t="shared" si="4"/>
-        <v>143.12</v>
+        <v>158.26999999999998</v>
       </c>
       <c r="M8">
         <v>-1.3333333333333263E-4</v>
@@ -10917,35 +10917,35 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="E9">
         <v>130</v>
       </c>
       <c r="F9">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>507</v>
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
-        <v>498.39999999999952</v>
+        <v>646.39999999999952</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>252.68879999999976</v>
+        <v>327.72479999999973</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>356.88</v>
+        <v>341.73</v>
       </c>
       <c r="K9">
         <v>500</v>
       </c>
       <c r="L9">
         <f t="shared" si="4"/>
-        <v>143.12</v>
+        <v>158.26999999999998</v>
       </c>
       <c r="M9">
         <v>-1.3333333333333263E-4</v>
@@ -10982,35 +10982,35 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="E10">
         <v>130</v>
       </c>
       <c r="F10">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>508</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>498.39999999999952</v>
+        <v>646.39999999999952</v>
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>253.18719999999976</v>
+        <v>328.37119999999976</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>356.88</v>
+        <v>341.73</v>
       </c>
       <c r="K10">
         <v>500</v>
       </c>
       <c r="L10">
         <f t="shared" si="4"/>
-        <v>143.12</v>
+        <v>158.26999999999998</v>
       </c>
       <c r="M10">
         <v>-1.3333333333333263E-4</v>
@@ -11050,35 +11050,35 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E11">
         <v>80</v>
       </c>
       <c r="F11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>509</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>329.01759999999973</v>
+        <v>373.80959999999982</v>
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K11">
         <v>500</v>
       </c>
       <c r="L11">
         <f t="shared" si="4"/>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M11">
         <v>-1.3333333333333263E-4</v>
@@ -11118,35 +11118,35 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E12">
         <v>80</v>
       </c>
       <c r="F12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>510</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>329.66399999999976</v>
+        <v>374.54399999999981</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K12">
         <v>500</v>
       </c>
       <c r="L12">
         <f t="shared" si="4"/>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M12">
         <v>-1.3333333333333263E-4</v>
@@ -11186,35 +11186,35 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E13">
         <v>80</v>
       </c>
       <c r="F13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>511</v>
       </c>
       <c r="H13">
         <f t="shared" si="2"/>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>330.31039999999973</v>
+        <v>375.27839999999981</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K13">
         <v>500</v>
       </c>
       <c r="L13">
         <f t="shared" si="4"/>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M13">
         <v>-1.3333333333333263E-4</v>
@@ -11254,35 +11254,35 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E14">
         <v>80</v>
       </c>
       <c r="F14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>512</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>330.95679999999976</v>
+        <v>376.0127999999998</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K14">
         <v>500</v>
       </c>
       <c r="L14">
         <f t="shared" si="4"/>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M14">
         <v>-1.3333333333333263E-4</v>
@@ -11322,35 +11322,35 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E15">
         <v>80</v>
       </c>
       <c r="F15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>513</v>
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
-        <v>331.60319999999979</v>
+        <v>376.74719999999985</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K15">
         <v>500</v>
       </c>
       <c r="L15">
         <f t="shared" si="4"/>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M15">
         <v>-1.3333333333333263E-4</v>
@@ -11390,35 +11390,35 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E16">
         <v>80</v>
       </c>
       <c r="F16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>514</v>
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>332.24959999999976</v>
+        <v>377.48159999999979</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K16">
         <v>500</v>
       </c>
       <c r="L16">
         <f t="shared" si="4"/>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M16">
         <v>-1.3333333333333263E-4</v>
@@ -11455,35 +11455,35 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E17">
         <v>80</v>
       </c>
       <c r="F17">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>515</v>
       </c>
       <c r="H17">
         <f t="shared" si="2"/>
-        <v>646.39999999999952</v>
+        <v>734.39999999999964</v>
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>332.89599999999979</v>
+        <v>378.21599999999984</v>
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
-        <v>341.73</v>
+        <v>322.08</v>
       </c>
       <c r="K17">
         <v>500</v>
       </c>
       <c r="L17">
         <f t="shared" si="4"/>
-        <v>158.26999999999998</v>
+        <v>177.92000000000002</v>
       </c>
       <c r="M17">
         <v>-1.3333333333333263E-4</v>
@@ -18737,18 +18737,18 @@
       </c>
       <c r="B2" s="35">
         <f>SUMIF(Wells!$C$2:$C$200,A2,Wells!$H$2:$H$200)</f>
-        <v>51320.000000000058</v>
+        <v>52108.000000000058</v>
       </c>
       <c r="C2" s="35">
         <f>SUMIF(Wells!$C$2:$C$200,A2,Wells!$I$2:$I$200)</f>
-        <v>29721.702399999984</v>
+        <v>30115.966399999983</v>
       </c>
       <c r="D2" s="35">
         <v>130</v>
       </c>
       <c r="E2">
         <f>COUNTIF(Wells!$C$2:$C$200,A2)</f>
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -18757,18 +18757,18 @@
       </c>
       <c r="B3" s="35">
         <f>SUMIF(Wells!$C$2:$C$200,A3,Wells!$H$2:$H$200)</f>
-        <v>21017.599999999999</v>
+        <v>20563.199999999997</v>
       </c>
       <c r="C3" s="35">
         <f>SUMIF(Wells!$C$2:$C$200,A3,Wells!$I$2:$I$200)</f>
-        <v>11431.188799999994</v>
+        <v>11210.615999999996</v>
       </c>
       <c r="D3" s="35">
         <v>79</v>
       </c>
       <c r="E3">
         <f>COUNTIF(Wells!$C$2:$C$200,A3)</f>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -18777,18 +18777,18 @@
       </c>
       <c r="B4" s="35">
         <f>SUMIF(Wells!$C$2:$C$200,A4,Wells!$H$2:$H$200)</f>
-        <v>14275.19999999999</v>
+        <v>15601.599999999991</v>
       </c>
       <c r="C4" s="35">
         <f>SUMIF(Wells!$C$2:$C$200,A4,Wells!$I$2:$I$200)</f>
-        <v>7589.6119999999946</v>
+        <v>8257.9807999999939</v>
       </c>
       <c r="D4" s="35">
         <v>130</v>
       </c>
       <c r="E4">
         <f>COUNTIF(Wells!$C$2:$C$200,A4)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -18797,11 +18797,11 @@
       </c>
       <c r="B5" s="36">
         <f>SUM(B2:B4)</f>
-        <v>86612.800000000047</v>
+        <v>88272.800000000047</v>
       </c>
       <c r="C5" s="36">
         <f>SUM(C2:C4)</f>
-        <v>48742.50319999997</v>
+        <v>49584.563199999975</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5">

</xml_diff>

<commit_message>
fixed sidebar width on different screen size, started session dependency remove
</commit_message>
<xml_diff>
--- a/lineup_app/static/xlgap.xlsx
+++ b/lineup_app/static/xlgap.xlsx
@@ -1799,11 +1799,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="220993408"/>
-        <c:axId val="220994944"/>
+        <c:axId val="206841728"/>
+        <c:axId val="206843264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="220993408"/>
+        <c:axId val="206841728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1813,12 +1813,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220994944"/>
+        <c:crossAx val="206843264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="220994944"/>
+        <c:axId val="206843264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1829,14 +1829,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220993408"/>
+        <c:crossAx val="206841728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>

</xml_diff>